<commit_message>
Removed "Coluna Certificate(Classificação Etária)" with no percentual, and kept only the percentual one. Added a few more columns frequency. Updated Readme.
</commit_message>
<xml_diff>
--- a/Resultados/frequencia_certificate.xlsx
+++ b/Resultados/frequencia_certificate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Frequency</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -454,6 +459,11 @@
       <c r="B2" t="n">
         <v>183</v>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>25.67%</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -464,6 +474,11 @@
       <c r="B3" t="n">
         <v>173</v>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>24.26%</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -474,6 +489,11 @@
       <c r="B4" t="n">
         <v>142</v>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>19.92%</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -484,6 +504,11 @@
       <c r="B5" t="n">
         <v>131</v>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>18.37%</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -494,6 +519,11 @@
       <c r="B6" t="n">
         <v>38</v>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5.33%</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -504,6 +534,11 @@
       <c r="B7" t="n">
         <v>19</v>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2.66%</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -514,6 +549,11 @@
       <c r="B8" t="n">
         <v>9</v>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.26%</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -524,6 +564,11 @@
       <c r="B9" t="n">
         <v>9</v>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1.26%</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -534,6 +579,11 @@
       <c r="B10" t="n">
         <v>6</v>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.84%</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -544,6 +594,11 @@
       <c r="B11" t="n">
         <v>1</v>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.14%</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -554,6 +609,11 @@
       <c r="B12" t="n">
         <v>1</v>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.14%</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -563,6 +623,11 @@
       </c>
       <c r="B13" t="n">
         <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.14%</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>